<commit_message>
add: CPZE, fix: some bags
</commit_message>
<xml_diff>
--- a/scripts/_misc/Data_SAS_fixed.xlsx
+++ b/scripts/_misc/Data_SAS_fixed.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -224,9 +224,6 @@
     <t xml:space="preserve">Comp Z</t>
   </si>
   <si>
-    <t xml:space="preserve">Comp_Z</t>
-  </si>
-  <si>
     <t xml:space="preserve">negative</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t xml:space="preserve">depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPZE</t>
   </si>
   <si>
     <t xml:space="preserve">А1</t>
@@ -404,13 +404,13 @@
     <t xml:space="preserve">А23</t>
   </si>
   <si>
-    <t xml:space="preserve">4,5</t>
+    <t xml:space="preserve">4.5</t>
   </si>
   <si>
     <t xml:space="preserve">А24</t>
   </si>
   <si>
-    <t xml:space="preserve">1,5</t>
+    <t xml:space="preserve">1.5</t>
   </si>
   <si>
     <t xml:space="preserve">А25</t>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t xml:space="preserve">п7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.5</t>
   </si>
   <si>
     <t xml:space="preserve">п15</t>
@@ -1295,25 +1292,25 @@
         <v>-4.85</v>
       </c>
       <c r="BR2" t="n">
-        <v>-3.85</v>
+        <v>35.35</v>
       </c>
       <c r="BS2" t="n">
-        <v>35.35</v>
+        <v>31</v>
       </c>
       <c r="BT2" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="BU2" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="BV2" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="BW2" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="BX2" t="n">
-        <v>17</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="3">
@@ -1525,25 +1522,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR3" t="n">
-        <v>-1.02</v>
+        <v>50.01</v>
       </c>
       <c r="BS3" t="n">
-        <v>50.01</v>
+        <v>23</v>
       </c>
       <c r="BT3" t="n">
+        <v>16</v>
+      </c>
+      <c r="BU3" t="n">
         <v>23</v>
       </c>
-      <c r="BU3" t="n">
-        <v>16</v>
-      </c>
       <c r="BV3" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="BW3" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BX3" t="n">
-        <v>15</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="4">
@@ -1755,25 +1752,25 @@
         <v>2.24</v>
       </c>
       <c r="BR4" t="n">
-        <v>-0.09</v>
+        <v>55.47</v>
       </c>
       <c r="BS4" t="n">
-        <v>55.47</v>
+        <v>29</v>
       </c>
       <c r="BT4" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="BU4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BV4" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BW4" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="BX4" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -1985,25 +1982,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR5" t="n">
-        <v>-1.42</v>
+        <v>50.16</v>
       </c>
       <c r="BS5" t="n">
-        <v>50.16</v>
+        <v>19</v>
       </c>
       <c r="BT5" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="BU5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="BV5" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="BW5" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BX5" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -2215,25 +2212,25 @@
         <v>0.34</v>
       </c>
       <c r="BR6" t="n">
-        <v>-1.53</v>
+        <v>51.16</v>
       </c>
       <c r="BS6" t="n">
-        <v>51.16</v>
+        <v>19</v>
       </c>
       <c r="BT6" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="BU6" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BV6" t="n">
         <v>17</v>
       </c>
       <c r="BW6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BX6" t="n">
-        <v>19</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="7">
@@ -2445,25 +2442,25 @@
         <v>1.4</v>
       </c>
       <c r="BR7" t="n">
-        <v>-0.27</v>
+        <v>54.16</v>
       </c>
       <c r="BS7" t="n">
-        <v>54.16</v>
+        <v>17</v>
       </c>
       <c r="BT7" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="BU7" t="n">
+        <v>12</v>
+      </c>
+      <c r="BV7" t="n">
         <v>10</v>
       </c>
-      <c r="BV7" t="n">
-        <v>12</v>
-      </c>
       <c r="BW7" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BX7" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -2675,25 +2672,25 @@
         <v>0.17</v>
       </c>
       <c r="BR8" t="n">
-        <v>-1.84</v>
+        <v>44.63</v>
       </c>
       <c r="BS8" t="n">
-        <v>44.63</v>
+        <v>19</v>
       </c>
       <c r="BT8" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="BU8" t="n">
         <v>13</v>
       </c>
       <c r="BV8" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="BW8" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="BX8" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -2905,25 +2902,25 @@
         <v>-0.8</v>
       </c>
       <c r="BR9" t="n">
-        <v>-1.51</v>
+        <v>42.98</v>
       </c>
       <c r="BS9" t="n">
-        <v>42.98</v>
+        <v>18</v>
       </c>
       <c r="BT9" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="BU9" t="n">
+        <v>13</v>
+      </c>
+      <c r="BV9" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW9" t="n">
         <v>12</v>
       </c>
-      <c r="BV9" t="n">
-        <v>13</v>
-      </c>
-      <c r="BW9" t="n">
-        <v>8</v>
-      </c>
       <c r="BX9" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -3135,25 +3132,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR10" t="n">
-        <v>-0.94</v>
+        <v>51.01</v>
       </c>
       <c r="BS10" t="n">
-        <v>51.01</v>
+        <v>16</v>
       </c>
       <c r="BT10" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="BU10" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BV10" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BW10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BX10" t="n">
-        <v>12</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="11">
@@ -3365,25 +3362,25 @@
         <v>0.17</v>
       </c>
       <c r="BR11" t="n">
-        <v>-0.69</v>
+        <v>52.59</v>
       </c>
       <c r="BS11" t="n">
-        <v>52.59</v>
+        <v>15</v>
       </c>
       <c r="BT11" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="BU11" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BV11" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW11" t="n">
         <v>11</v>
       </c>
-      <c r="BW11" t="n">
-        <v>10</v>
-      </c>
       <c r="BX11" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -3595,25 +3592,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR12" t="n">
-        <v>-1.87</v>
+        <v>46.91</v>
       </c>
       <c r="BS12" t="n">
-        <v>46.91</v>
+        <v>16</v>
       </c>
       <c r="BT12" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="BU12" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BV12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="BW12" t="n">
         <v>10</v>
       </c>
       <c r="BX12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -3825,25 +3822,25 @@
         <v>0.8</v>
       </c>
       <c r="BR13" t="n">
-        <v>-1.01</v>
+        <v>51.5</v>
       </c>
       <c r="BS13" t="n">
-        <v>51.5</v>
+        <v>21</v>
       </c>
       <c r="BT13" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="BU13" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BV13" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BW13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="BX13" t="n">
-        <v>10</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="14">
@@ -4055,25 +4052,25 @@
         <v>-6.22</v>
       </c>
       <c r="BR14" t="n">
-        <v>-3.03</v>
+        <v>44.48</v>
       </c>
       <c r="BS14" t="n">
-        <v>44.48</v>
+        <v>25</v>
       </c>
       <c r="BT14" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="BU14" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="BV14" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW14" t="n">
         <v>18</v>
       </c>
-      <c r="BW14" t="n">
-        <v>8</v>
-      </c>
       <c r="BX14" t="n">
-        <v>18</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="15">
@@ -4285,25 +4282,25 @@
         <v>-5.19</v>
       </c>
       <c r="BR15" t="n">
-        <v>-3.54</v>
+        <v>39.57</v>
       </c>
       <c r="BS15" t="n">
-        <v>39.57</v>
+        <v>12</v>
       </c>
       <c r="BT15" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="BU15" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="BV15" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BW15" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="BX15" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -4515,25 +4512,25 @@
         <v>-4.2</v>
       </c>
       <c r="BR16" t="n">
-        <v>-4.41</v>
+        <v>35.06</v>
       </c>
       <c r="BS16" t="n">
-        <v>35.06</v>
+        <v>20</v>
       </c>
       <c r="BT16" t="n">
+        <v>14</v>
+      </c>
+      <c r="BU16" t="n">
+        <v>17</v>
+      </c>
+      <c r="BV16" t="n">
+        <v>11</v>
+      </c>
+      <c r="BW16" t="n">
         <v>20</v>
       </c>
-      <c r="BU16" t="n">
-        <v>14</v>
-      </c>
-      <c r="BV16" t="n">
-        <v>17</v>
-      </c>
-      <c r="BW16" t="n">
-        <v>11</v>
-      </c>
       <c r="BX16" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -4745,25 +4742,25 @@
         <v>1.74</v>
       </c>
       <c r="BR17" t="n">
-        <v>-0.04</v>
+        <v>56.8</v>
       </c>
       <c r="BS17" t="n">
-        <v>56.8</v>
+        <v>18</v>
       </c>
       <c r="BT17" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="BU17" t="n">
+        <v>11</v>
+      </c>
+      <c r="BV17" t="n">
         <v>7</v>
       </c>
-      <c r="BV17" t="n">
-        <v>11</v>
-      </c>
       <c r="BW17" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BX17" t="n">
-        <v>15</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="18">
@@ -4975,25 +4972,25 @@
         <v>-1.35</v>
       </c>
       <c r="BR18" t="n">
-        <v>-2.91</v>
+        <v>40.23</v>
       </c>
       <c r="BS18" t="n">
-        <v>40.23</v>
+        <v>24</v>
       </c>
       <c r="BT18" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="BU18" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="BV18" t="n">
+        <v>11</v>
+      </c>
+      <c r="BW18" t="n">
         <v>17</v>
       </c>
-      <c r="BW18" t="n">
-        <v>11</v>
-      </c>
       <c r="BX18" t="n">
-        <v>17</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="19">
@@ -5205,25 +5202,25 @@
         <v>-1.38</v>
       </c>
       <c r="BR19" t="n">
-        <v>-1.55</v>
+        <v>50.47</v>
       </c>
       <c r="BS19" t="n">
-        <v>50.47</v>
+        <v>14</v>
       </c>
       <c r="BT19" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BU19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="BV19" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BW19" t="n">
         <v>12</v>
       </c>
       <c r="BX19" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -5435,25 +5432,25 @@
         <v>-1.26</v>
       </c>
       <c r="BR20" t="n">
-        <v>-1.93</v>
+        <v>48.11</v>
       </c>
       <c r="BS20" t="n">
-        <v>48.11</v>
+        <v>19</v>
       </c>
       <c r="BT20" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="BU20" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="BV20" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="BW20" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BX20" t="n">
-        <v>12</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="21">
@@ -5665,25 +5662,25 @@
         <v>1.74</v>
       </c>
       <c r="BR21" t="n">
-        <v>-0.53</v>
+        <v>59.54</v>
       </c>
       <c r="BS21" t="n">
-        <v>59.54</v>
+        <v>17</v>
       </c>
       <c r="BT21" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="BU21" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="BV21" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW21" t="n">
         <v>11</v>
       </c>
-      <c r="BW21" t="n">
-        <v>8</v>
-      </c>
       <c r="BX21" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -5895,25 +5892,25 @@
         <v>-2.46</v>
       </c>
       <c r="BR22" t="n">
-        <v>-3.37</v>
+        <v>34.26</v>
       </c>
       <c r="BS22" t="n">
-        <v>34.26</v>
+        <v>20</v>
       </c>
       <c r="BT22" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BU22" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="BV22" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BW22" t="n">
         <v>14</v>
       </c>
       <c r="BX22" t="n">
-        <v>14</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="23">
@@ -6125,25 +6122,25 @@
         <v>-0.66</v>
       </c>
       <c r="BR23" t="n">
-        <v>0.08</v>
+        <v>58.84</v>
       </c>
       <c r="BS23" t="n">
-        <v>58.84</v>
+        <v>19</v>
       </c>
       <c r="BT23" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="BU23" t="n">
+        <v>15</v>
+      </c>
+      <c r="BV23" t="n">
         <v>11</v>
       </c>
-      <c r="BV23" t="n">
-        <v>15</v>
-      </c>
       <c r="BW23" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="BX23" t="n">
-        <v>17</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="24">
@@ -6355,25 +6352,25 @@
         <v>-2.99</v>
       </c>
       <c r="BR24" t="n">
-        <v>-3.46</v>
+        <v>35.76</v>
       </c>
       <c r="BS24" t="n">
-        <v>35.76</v>
+        <v>25</v>
       </c>
       <c r="BT24" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="BU24" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="BV24" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="BW24" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="BX24" t="n">
-        <v>16</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="25">
@@ -6585,25 +6582,25 @@
         <v>-0.79</v>
       </c>
       <c r="BR25" t="n">
-        <v>-2.34</v>
+        <v>42.17</v>
       </c>
       <c r="BS25" t="n">
-        <v>42.17</v>
+        <v>17</v>
       </c>
       <c r="BT25" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU25" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="BV25" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="BW25" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="BX25" t="n">
-        <v>19</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26">
@@ -6815,25 +6812,25 @@
         <v>-6.65</v>
       </c>
       <c r="BR26" t="n">
-        <v>-4.31</v>
+        <v>33.83</v>
       </c>
       <c r="BS26" t="n">
-        <v>33.83</v>
+        <v>21</v>
       </c>
       <c r="BT26" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="BU26" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="BV26" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="BW26" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="BX26" t="n">
-        <v>15</v>
+        <v>9.01</v>
       </c>
     </row>
     <row r="27">
@@ -7045,25 +7042,25 @@
         <v>-5.01</v>
       </c>
       <c r="BR27" t="n">
-        <v>-2.9</v>
+        <v>44.33</v>
       </c>
       <c r="BS27" t="n">
-        <v>44.33</v>
+        <v>17</v>
       </c>
       <c r="BT27" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU27" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="BV27" t="n">
+        <v>11</v>
+      </c>
+      <c r="BW27" t="n">
         <v>15</v>
       </c>
-      <c r="BW27" t="n">
-        <v>11</v>
-      </c>
       <c r="BX27" t="n">
-        <v>15</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="28">
@@ -7275,25 +7272,25 @@
         <v>-0.66</v>
       </c>
       <c r="BR28" t="n">
-        <v>-0.02</v>
+        <v>60.09</v>
       </c>
       <c r="BS28" t="n">
-        <v>60.09</v>
+        <v>22</v>
       </c>
       <c r="BT28" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="BU28" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BV28" t="n">
+        <v>6</v>
+      </c>
+      <c r="BW28" t="n">
         <v>11</v>
       </c>
-      <c r="BW28" t="n">
-        <v>6</v>
-      </c>
       <c r="BX28" t="n">
-        <v>11</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="29">
@@ -7505,25 +7502,25 @@
         <v>1.14</v>
       </c>
       <c r="BR29" t="n">
-        <v>-1.06</v>
+        <v>50.06</v>
       </c>
       <c r="BS29" t="n">
-        <v>50.06</v>
+        <v>27</v>
       </c>
       <c r="BT29" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="BU29" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BV29" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BW29" t="n">
         <v>15</v>
       </c>
       <c r="BX29" t="n">
-        <v>15</v>
+        <v>7.49</v>
       </c>
     </row>
     <row r="30">
@@ -7735,25 +7732,25 @@
         <v>0.69</v>
       </c>
       <c r="BR30" t="n">
-        <v>-0.77</v>
+        <v>50.74</v>
       </c>
       <c r="BS30" t="n">
-        <v>50.74</v>
+        <v>18</v>
       </c>
       <c r="BT30" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU30" t="n">
+        <v>12</v>
+      </c>
+      <c r="BV30" t="n">
+        <v>11</v>
+      </c>
+      <c r="BW30" t="n">
         <v>18</v>
       </c>
-      <c r="BU30" t="n">
-        <v>10</v>
-      </c>
-      <c r="BV30" t="n">
-        <v>12</v>
-      </c>
-      <c r="BW30" t="n">
-        <v>11</v>
-      </c>
       <c r="BX30" t="n">
-        <v>18</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="31">
@@ -7965,25 +7962,25 @@
         <v>-0.06</v>
       </c>
       <c r="BR31" t="n">
-        <v>-0.59</v>
+        <v>53.11</v>
       </c>
       <c r="BS31" t="n">
-        <v>53.11</v>
+        <v>23</v>
       </c>
       <c r="BT31" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="BU31" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="BV31" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="BW31" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="BX31" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -8195,25 +8192,25 @@
         <v>0.22</v>
       </c>
       <c r="BR32" t="n">
-        <v>-3.01</v>
+        <v>41.69</v>
       </c>
       <c r="BS32" t="n">
-        <v>41.69</v>
+        <v>18</v>
       </c>
       <c r="BT32" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="BU32" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="BV32" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BW32" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BX32" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -8425,25 +8422,25 @@
         <v>0.17</v>
       </c>
       <c r="BR33" t="n">
-        <v>-2.52</v>
+        <v>47.79</v>
       </c>
       <c r="BS33" t="n">
-        <v>47.79</v>
+        <v>19</v>
       </c>
       <c r="BT33" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="BU33" t="n">
+        <v>14</v>
+      </c>
+      <c r="BV33" t="n">
+        <v>11</v>
+      </c>
+      <c r="BW33" t="n">
         <v>12</v>
       </c>
-      <c r="BV33" t="n">
-        <v>14</v>
-      </c>
-      <c r="BW33" t="n">
-        <v>11</v>
-      </c>
       <c r="BX33" t="n">
-        <v>12</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="34">
@@ -8655,25 +8652,25 @@
         <v>-0.23</v>
       </c>
       <c r="BR34" t="n">
-        <v>-3.77</v>
+        <v>38.45</v>
       </c>
       <c r="BS34" t="n">
-        <v>38.45</v>
+        <v>17</v>
       </c>
       <c r="BT34" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU34" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BV34" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BW34" t="n">
         <v>12</v>
       </c>
       <c r="BX34" t="n">
-        <v>12</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="35">
@@ -8885,25 +8882,25 @@
         <v>-1.54</v>
       </c>
       <c r="BR35" t="n">
-        <v>-0.45</v>
+        <v>62.18</v>
       </c>
       <c r="BS35" t="n">
-        <v>62.18</v>
+        <v>17</v>
       </c>
       <c r="BT35" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU35" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BV35" t="n">
         <v>13</v>
       </c>
       <c r="BW35" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BX35" t="n">
-        <v>12</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="36">
@@ -9115,25 +9112,25 @@
         <v>0.17</v>
       </c>
       <c r="BR36" t="n">
-        <v>-1.65</v>
+        <v>47.37</v>
       </c>
       <c r="BS36" t="n">
-        <v>47.37</v>
+        <v>17</v>
       </c>
       <c r="BT36" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU36" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BV36" t="n">
+        <v>11</v>
+      </c>
+      <c r="BW36" t="n">
         <v>13</v>
       </c>
-      <c r="BW36" t="n">
-        <v>11</v>
-      </c>
       <c r="BX36" t="n">
-        <v>13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="37">
@@ -9345,25 +9342,25 @@
         <v>1.07</v>
       </c>
       <c r="BR37" t="n">
-        <v>-0.94</v>
+        <v>50.15</v>
       </c>
       <c r="BS37" t="n">
-        <v>50.15</v>
+        <v>17</v>
       </c>
       <c r="BT37" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="BU37" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BV37" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="BW37" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BX37" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -9575,25 +9572,25 @@
         <v>2.24</v>
       </c>
       <c r="BR38" t="n">
-        <v>-2.99</v>
+        <v>34.86</v>
       </c>
       <c r="BS38" t="n">
-        <v>34.86</v>
+        <v>17</v>
       </c>
       <c r="BT38" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU38" t="n">
+        <v>14</v>
+      </c>
+      <c r="BV38" t="n">
         <v>9</v>
       </c>
-      <c r="BV38" t="n">
-        <v>14</v>
-      </c>
       <c r="BW38" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BX38" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -9805,25 +9802,25 @@
         <v>-2.13</v>
       </c>
       <c r="BR39" t="n">
-        <v>-0.92</v>
+        <v>59.18</v>
       </c>
       <c r="BS39" t="n">
-        <v>59.18</v>
+        <v>19</v>
       </c>
       <c r="BT39" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="BU39" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BV39" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BW39" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BX39" t="n">
-        <v>15</v>
+        <v>7.49</v>
       </c>
     </row>
     <row r="40">
@@ -9843,7 +9840,7 @@
         <v>126</v>
       </c>
       <c r="F40" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G40" t="s">
         <v>91</v>
@@ -10035,30 +10032,30 @@
         <v>0.17</v>
       </c>
       <c r="BR40" t="n">
-        <v>-1.37</v>
+        <v>51.15</v>
       </c>
       <c r="BS40" t="n">
-        <v>51.15</v>
+        <v>15</v>
       </c>
       <c r="BT40" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="BU40" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BV40" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BW40" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="BX40" t="n">
-        <v>12</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" t="s">
         <v>77</v>
@@ -10265,30 +10262,30 @@
         <v>-2.46</v>
       </c>
       <c r="BR41" t="n">
-        <v>-3.57</v>
+        <v>32.54</v>
       </c>
       <c r="BS41" t="n">
-        <v>32.54</v>
+        <v>16</v>
       </c>
       <c r="BT41" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BU41" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="BV41" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BW41" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="BX41" t="n">
-        <v>14</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
         <v>77</v>
@@ -10495,30 +10492,30 @@
         <v>-2.45</v>
       </c>
       <c r="BR42" t="n">
-        <v>-2.03</v>
+        <v>48.31</v>
       </c>
       <c r="BS42" t="n">
-        <v>48.31</v>
+        <v>17</v>
       </c>
       <c r="BT42" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU42" t="n">
+        <v>11</v>
+      </c>
+      <c r="BV42" t="n">
         <v>9</v>
       </c>
-      <c r="BV42" t="n">
-        <v>11</v>
-      </c>
       <c r="BW42" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BX42" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
         <v>88</v>
@@ -10533,7 +10530,7 @@
         <v>126</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G43" t="s">
         <v>91</v>
@@ -10725,30 +10722,30 @@
         <v>0.34</v>
       </c>
       <c r="BR43" t="n">
-        <v>-2.48</v>
+        <v>40.95</v>
       </c>
       <c r="BS43" t="n">
-        <v>40.95</v>
+        <v>18</v>
       </c>
       <c r="BT43" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="BU43" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BV43" t="n">
+        <v>7</v>
+      </c>
+      <c r="BW43" t="n">
         <v>12</v>
       </c>
-      <c r="BW43" t="n">
-        <v>7</v>
-      </c>
       <c r="BX43" t="n">
-        <v>12</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
         <v>77</v>
@@ -10955,30 +10952,30 @@
         <v>0.3</v>
       </c>
       <c r="BR44" t="n">
-        <v>-2.47</v>
+        <v>39.44</v>
       </c>
       <c r="BS44" t="n">
-        <v>39.44</v>
+        <v>18</v>
       </c>
       <c r="BT44" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="BU44" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="BV44" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="BW44" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BX44" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" t="s">
         <v>88</v>
@@ -10990,7 +10987,7 @@
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F45" t="s">
         <v>79</v>
@@ -11185,30 +11182,30 @@
         <v>-0.37</v>
       </c>
       <c r="BR45" t="n">
-        <v>-3.86</v>
+        <v>28.72</v>
       </c>
       <c r="BS45" t="n">
-        <v>28.72</v>
+        <v>21</v>
       </c>
       <c r="BT45" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="BU45" t="n">
+        <v>11</v>
+      </c>
+      <c r="BV45" t="n">
         <v>6</v>
       </c>
-      <c r="BV45" t="n">
-        <v>11</v>
-      </c>
       <c r="BW45" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="BX45" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B46" t="s">
         <v>88</v>
@@ -11415,30 +11412,30 @@
         <v>-1.38</v>
       </c>
       <c r="BR46" t="n">
-        <v>-4.13</v>
+        <v>29.46</v>
       </c>
       <c r="BS46" t="n">
-        <v>29.46</v>
+        <v>15</v>
       </c>
       <c r="BT46" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BU46" t="n">
+        <v>10</v>
+      </c>
+      <c r="BV46" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW46" t="n">
+        <v>11</v>
+      </c>
+      <c r="BX46" t="n">
         <v>6</v>
-      </c>
-      <c r="BV46" t="n">
-        <v>10</v>
-      </c>
-      <c r="BW46" t="n">
-        <v>8</v>
-      </c>
-      <c r="BX46" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B47" t="s">
         <v>88</v>
@@ -11450,10 +11447,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G47" t="s">
         <v>80</v>
@@ -11645,30 +11642,30 @@
         <v>-0.96</v>
       </c>
       <c r="BR47" t="n">
-        <v>-4.29</v>
+        <v>27.78</v>
       </c>
       <c r="BS47" t="n">
-        <v>27.78</v>
+        <v>22</v>
       </c>
       <c r="BT47" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="BU47" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BV47" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BW47" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BX47" t="n">
-        <v>15</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B48" t="s">
         <v>77</v>
@@ -11875,30 +11872,30 @@
         <v>-1.8</v>
       </c>
       <c r="BR48" t="n">
-        <v>-1.58</v>
+        <v>36.32</v>
       </c>
       <c r="BS48" t="n">
-        <v>36.32</v>
+        <v>13</v>
       </c>
       <c r="BT48" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="BU48" t="n">
+        <v>14</v>
+      </c>
+      <c r="BV48" t="n">
         <v>8</v>
       </c>
-      <c r="BV48" t="n">
-        <v>14</v>
-      </c>
       <c r="BW48" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BX48" t="n">
-        <v>9</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
         <v>88</v>
@@ -12105,30 +12102,30 @@
         <v>0.17</v>
       </c>
       <c r="BR49" t="n">
-        <v>0.06</v>
+        <v>57.89</v>
       </c>
       <c r="BS49" t="n">
-        <v>57.89</v>
+        <v>25</v>
       </c>
       <c r="BT49" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="BU49" t="n">
+        <v>14</v>
+      </c>
+      <c r="BV49" t="n">
         <v>6</v>
       </c>
-      <c r="BV49" t="n">
-        <v>14</v>
-      </c>
       <c r="BW49" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="BX49" t="n">
-        <v>17</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B50" t="s">
         <v>88</v>
@@ -12335,30 +12332,30 @@
         <v>0.69</v>
       </c>
       <c r="BR50" t="n">
-        <v>-1.41</v>
+        <v>46.31</v>
       </c>
       <c r="BS50" t="n">
-        <v>46.31</v>
+        <v>17</v>
       </c>
       <c r="BT50" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="BU50" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="BV50" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BW50" t="n">
         <v>10</v>
       </c>
       <c r="BX50" t="n">
-        <v>10</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B51" t="s">
         <v>77</v>
@@ -12565,30 +12562,30 @@
         <v>-2.13</v>
       </c>
       <c r="BR51" t="n">
-        <v>-5.56</v>
+        <v>14.19</v>
       </c>
       <c r="BS51" t="n">
-        <v>14.19</v>
+        <v>21</v>
       </c>
       <c r="BT51" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="BU51" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="BV51" t="n">
         <v>14</v>
       </c>
       <c r="BW51" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BX51" t="n">
-        <v>13</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
         <v>88</v>
@@ -12795,30 +12792,30 @@
         <v>0.21</v>
       </c>
       <c r="BR52" t="n">
-        <v>-2.2</v>
+        <v>38.96</v>
       </c>
       <c r="BS52" t="n">
-        <v>38.96</v>
+        <v>13</v>
       </c>
       <c r="BT52" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU52" t="n">
         <v>13</v>
       </c>
-      <c r="BU52" t="n">
-        <v>8</v>
-      </c>
       <c r="BV52" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BW52" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BX52" t="n">
-        <v>9</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B53" t="s">
         <v>77</v>
@@ -13025,30 +13022,30 @@
         <v>-1.35</v>
       </c>
       <c r="BR53" t="n">
-        <v>-4.77</v>
+        <v>28.31</v>
       </c>
       <c r="BS53" t="n">
-        <v>28.31</v>
+        <v>26</v>
       </c>
       <c r="BT53" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="BU53" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="BV53" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="BW53" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BX53" t="n">
-        <v>7</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
         <v>88</v>
@@ -13255,30 +13252,30 @@
         <v>-0.23</v>
       </c>
       <c r="BR54" t="n">
-        <v>-0.4</v>
+        <v>54.65</v>
       </c>
       <c r="BS54" t="n">
-        <v>54.65</v>
+        <v>15</v>
       </c>
       <c r="BT54" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="BU54" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="BV54" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW54" t="n">
         <v>13</v>
       </c>
-      <c r="BW54" t="n">
-        <v>8</v>
-      </c>
       <c r="BX54" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" t="s">
         <v>77</v>
@@ -13485,25 +13482,25 @@
         <v>-0.8</v>
       </c>
       <c r="BR55" t="n">
-        <v>-3.53</v>
+        <v>38.14</v>
       </c>
       <c r="BS55" t="n">
-        <v>38.14</v>
+        <v>15</v>
       </c>
       <c r="BT55" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="BU55" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="BV55" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BW55" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BX55" t="n">
-        <v>8</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="56">
@@ -13715,25 +13712,25 @@
         <v>-2.46</v>
       </c>
       <c r="BR56" t="n">
-        <v>-2.77</v>
+        <v>39.63</v>
       </c>
       <c r="BS56" t="n">
-        <v>39.63</v>
+        <v>21</v>
       </c>
       <c r="BT56" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="BU56" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BV56" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW56" t="n">
         <v>13</v>
       </c>
-      <c r="BW56" t="n">
-        <v>9</v>
-      </c>
       <c r="BX56" t="n">
-        <v>13</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="57">
@@ -13945,25 +13942,25 @@
         <v>-1.9</v>
       </c>
       <c r="BR57" t="n">
-        <v>-0.24</v>
+        <v>52.75</v>
       </c>
       <c r="BS57" t="n">
-        <v>52.75</v>
+        <v>17</v>
       </c>
       <c r="BT57" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="BU57" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BV57" t="n">
         <v>12</v>
       </c>
       <c r="BW57" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BX57" t="n">
-        <v>13</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="58">
@@ -14175,13 +14172,13 @@
         <v>2.24</v>
       </c>
       <c r="BR58" t="n">
-        <v>-0.79</v>
+        <v>51.73</v>
       </c>
       <c r="BS58" t="n">
-        <v>51.73</v>
+        <v>17</v>
       </c>
       <c r="BT58" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="BU58" t="n">
         <v>10</v>
@@ -14190,10 +14187,10 @@
         <v>10</v>
       </c>
       <c r="BW58" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BX58" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -14405,25 +14402,25 @@
         <v>0.3</v>
       </c>
       <c r="BR59" t="n">
-        <v>-0.06</v>
+        <v>59.06</v>
       </c>
       <c r="BS59" t="n">
-        <v>59.06</v>
+        <v>11</v>
       </c>
       <c r="BT59" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BU59" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BV59" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BW59" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BX59" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -14635,25 +14632,25 @@
         <v>-1.93</v>
       </c>
       <c r="BR60" t="n">
-        <v>-1.38</v>
+        <v>53.4</v>
       </c>
       <c r="BS60" t="n">
-        <v>53.4</v>
+        <v>16</v>
       </c>
       <c r="BT60" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="BU60" t="n">
+        <v>12</v>
+      </c>
+      <c r="BV60" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW60" t="n">
         <v>10</v>
       </c>
-      <c r="BV60" t="n">
-        <v>12</v>
-      </c>
-      <c r="BW60" t="n">
-        <v>9</v>
-      </c>
       <c r="BX60" t="n">
-        <v>10</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="61">
@@ -14865,25 +14862,25 @@
         <v>1.95</v>
       </c>
       <c r="BR61" t="n">
-        <v>0.32</v>
+        <v>58.02</v>
       </c>
       <c r="BS61" t="n">
-        <v>58.02</v>
+        <v>13</v>
       </c>
       <c r="BT61" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BU61" t="n">
+        <v>9</v>
+      </c>
+      <c r="BV61" t="n">
         <v>7</v>
       </c>
-      <c r="BV61" t="n">
+      <c r="BW61" t="n">
         <v>9</v>
       </c>
-      <c r="BW61" t="n">
-        <v>7</v>
-      </c>
       <c r="BX61" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
@@ -15095,25 +15092,25 @@
         <v>0.17</v>
       </c>
       <c r="BR62" t="n">
-        <v>-1.27</v>
+        <v>49.74</v>
       </c>
       <c r="BS62" t="n">
-        <v>49.74</v>
+        <v>13</v>
       </c>
       <c r="BT62" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="BU62" t="n">
+        <v>10</v>
+      </c>
+      <c r="BV62" t="n">
+        <v>6</v>
+      </c>
+      <c r="BW62" t="n">
         <v>8</v>
       </c>
-      <c r="BV62" t="n">
-        <v>10</v>
-      </c>
-      <c r="BW62" t="n">
-        <v>6</v>
-      </c>
       <c r="BX62" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -15325,25 +15322,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR63" t="n">
-        <v>-1.01</v>
+        <v>47.36</v>
       </c>
       <c r="BS63" t="n">
-        <v>47.36</v>
+        <v>11</v>
       </c>
       <c r="BT63" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BU63" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="BV63" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BW63" t="n">
         <v>8</v>
       </c>
       <c r="BX63" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -15555,25 +15552,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR64" t="n">
-        <v>-0.56</v>
+        <v>54.73</v>
       </c>
       <c r="BS64" t="n">
-        <v>54.73</v>
+        <v>12</v>
       </c>
       <c r="BT64" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="BU64" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BV64" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BW64" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BX64" t="n">
-        <v>9</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="65">
@@ -15785,25 +15782,25 @@
         <v>0.17</v>
       </c>
       <c r="BR65" t="n">
-        <v>-1.33</v>
+        <v>46.65</v>
       </c>
       <c r="BS65" t="n">
-        <v>46.65</v>
+        <v>12</v>
       </c>
       <c r="BT65" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="BU65" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BV65" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BW65" t="n">
         <v>9</v>
       </c>
       <c r="BX65" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -16015,25 +16012,25 @@
         <v>-0.25</v>
       </c>
       <c r="BR66" t="n">
-        <v>-1.15</v>
+        <v>52.01</v>
       </c>
       <c r="BS66" t="n">
-        <v>52.01</v>
+        <v>9</v>
       </c>
       <c r="BT66" t="n">
+        <v>6</v>
+      </c>
+      <c r="BU66" t="n">
+        <v>7</v>
+      </c>
+      <c r="BV66" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW66" t="n">
         <v>9</v>
       </c>
-      <c r="BU66" t="n">
-        <v>6</v>
-      </c>
-      <c r="BV66" t="n">
-        <v>7</v>
-      </c>
-      <c r="BW66" t="n">
-        <v>10</v>
-      </c>
       <c r="BX66" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -16245,25 +16242,25 @@
         <v>0.8</v>
       </c>
       <c r="BR67" t="n">
-        <v>-0.65</v>
+        <v>54.93</v>
       </c>
       <c r="BS67" t="n">
-        <v>54.93</v>
+        <v>18</v>
       </c>
       <c r="BT67" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="BU67" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="BV67" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="BW67" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BX67" t="n">
-        <v>11</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="68">
@@ -16475,25 +16472,25 @@
         <v>-3.88</v>
       </c>
       <c r="BR68" t="n">
-        <v>-2.12</v>
+        <v>48.47</v>
       </c>
       <c r="BS68" t="n">
-        <v>48.47</v>
+        <v>14</v>
       </c>
       <c r="BT68" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="BU68" t="n">
+        <v>13</v>
+      </c>
+      <c r="BV68" t="n">
         <v>8</v>
       </c>
-      <c r="BV68" t="n">
-        <v>13</v>
-      </c>
       <c r="BW68" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BX68" t="n">
-        <v>12</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="69">
@@ -16705,25 +16702,25 @@
         <v>-4.09</v>
       </c>
       <c r="BR69" t="n">
-        <v>-3.59</v>
+        <v>37.01</v>
       </c>
       <c r="BS69" t="n">
-        <v>37.01</v>
+        <v>12</v>
       </c>
       <c r="BT69" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="BU69" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BV69" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BW69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BX69" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
@@ -16935,25 +16932,25 @@
         <v>-3.64</v>
       </c>
       <c r="BR70" t="n">
-        <v>-3.9</v>
+        <v>37.85</v>
       </c>
       <c r="BS70" t="n">
-        <v>37.85</v>
+        <v>13</v>
       </c>
       <c r="BT70" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="BU70" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="BV70" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="BW70" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BX70" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -17165,25 +17162,25 @@
         <v>1.74</v>
       </c>
       <c r="BR71" t="n">
-        <v>0.52</v>
+        <v>60.51</v>
       </c>
       <c r="BS71" t="n">
-        <v>60.51</v>
+        <v>16</v>
       </c>
       <c r="BT71" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="BU71" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="BV71" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BW71" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="BX71" t="n">
-        <v>12</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="72">
@@ -17395,25 +17392,25 @@
         <v>-0.8</v>
       </c>
       <c r="BR72" t="n">
-        <v>-2</v>
+        <v>45.42</v>
       </c>
       <c r="BS72" t="n">
-        <v>45.42</v>
+        <v>22</v>
       </c>
       <c r="BT72" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="BU72" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="BV72" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="BW72" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BX72" t="n">
-        <v>11</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="73">
@@ -17625,19 +17622,19 @@
         <v>-0.87</v>
       </c>
       <c r="BR73" t="n">
-        <v>-1.85</v>
+        <v>47.39</v>
       </c>
       <c r="BS73" t="n">
-        <v>47.39</v>
+        <v>8</v>
       </c>
       <c r="BT73" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="BU73" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BV73" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="BW73" t="n">
         <v>6</v>
@@ -17855,25 +17852,25 @@
         <v>-0.06</v>
       </c>
       <c r="BR74" t="n">
-        <v>-0.62</v>
+        <v>56.37</v>
       </c>
       <c r="BS74" t="n">
-        <v>56.37</v>
+        <v>10</v>
       </c>
       <c r="BT74" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="BU74" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BV74" t="n">
         <v>5</v>
       </c>
       <c r="BW74" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BX74" t="n">
-        <v>8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="75">
@@ -18085,25 +18082,25 @@
         <v>0.54</v>
       </c>
       <c r="BR75" t="n">
-        <v>-1.25</v>
+        <v>50.93</v>
       </c>
       <c r="BS75" t="n">
-        <v>50.93</v>
+        <v>13</v>
       </c>
       <c r="BT75" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="BU75" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BV75" t="n">
+        <v>5</v>
+      </c>
+      <c r="BW75" t="n">
         <v>6</v>
       </c>
-      <c r="BW75" t="n">
-        <v>5</v>
-      </c>
       <c r="BX75" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
@@ -18315,25 +18312,25 @@
         <v>-4.25</v>
       </c>
       <c r="BR76" t="n">
-        <v>-3.37</v>
+        <v>39.82</v>
       </c>
       <c r="BS76" t="n">
-        <v>39.82</v>
+        <v>9</v>
       </c>
       <c r="BT76" t="n">
         <v>9</v>
       </c>
       <c r="BU76" t="n">
+        <v>10</v>
+      </c>
+      <c r="BV76" t="n">
         <v>9</v>
       </c>
-      <c r="BV76" t="n">
-        <v>10</v>
-      </c>
       <c r="BW76" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BX76" t="n">
-        <v>11</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="77">
@@ -18545,25 +18542,25 @@
         <v>1.14</v>
       </c>
       <c r="BR77" t="n">
-        <v>-0.68</v>
+        <v>56.57</v>
       </c>
       <c r="BS77" t="n">
-        <v>56.57</v>
+        <v>13</v>
       </c>
       <c r="BT77" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BU77" t="n">
+        <v>10</v>
+      </c>
+      <c r="BV77" t="n">
         <v>7</v>
       </c>
-      <c r="BV77" t="n">
+      <c r="BW77" t="n">
         <v>10</v>
       </c>
-      <c r="BW77" t="n">
-        <v>7</v>
-      </c>
       <c r="BX77" t="n">
-        <v>10</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="78">
@@ -18775,25 +18772,25 @@
         <v>1.4</v>
       </c>
       <c r="BR78" t="n">
-        <v>-1.53</v>
+        <v>44.43</v>
       </c>
       <c r="BS78" t="n">
-        <v>44.43</v>
+        <v>14</v>
       </c>
       <c r="BT78" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="BU78" t="n">
+        <v>8</v>
+      </c>
+      <c r="BV78" t="n">
         <v>6</v>
       </c>
-      <c r="BV78" t="n">
-        <v>8</v>
-      </c>
       <c r="BW78" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="BX78" t="n">
-        <v>10</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="79">
@@ -19005,25 +19002,25 @@
         <v>0.55</v>
       </c>
       <c r="BR79" t="n">
-        <v>-2.58</v>
+        <v>38.96</v>
       </c>
       <c r="BS79" t="n">
-        <v>38.96</v>
+        <v>15</v>
       </c>
       <c r="BT79" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="BU79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BV79" t="n">
         <v>7</v>
       </c>
       <c r="BW79" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="BX79" t="n">
-        <v>11</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="80">
@@ -19235,25 +19232,25 @@
         <v>-3.05</v>
       </c>
       <c r="BR80" t="n">
-        <v>-3.26</v>
+        <v>36.73</v>
       </c>
       <c r="BS80" t="n">
-        <v>36.73</v>
+        <v>12</v>
       </c>
       <c r="BT80" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="BU80" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="BV80" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BW80" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BX80" t="n">
-        <v>10</v>
+        <v>9.01</v>
       </c>
     </row>
     <row r="81">
@@ -19465,25 +19462,25 @@
         <v>-2.42</v>
       </c>
       <c r="BR81" t="n">
-        <v>-1.65</v>
+        <v>49.61</v>
       </c>
       <c r="BS81" t="n">
-        <v>49.61</v>
+        <v>11</v>
       </c>
       <c r="BT81" t="n">
+        <v>6</v>
+      </c>
+      <c r="BU81" t="n">
         <v>11</v>
       </c>
-      <c r="BU81" t="n">
-        <v>6</v>
-      </c>
       <c r="BV81" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BW81" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="BX81" t="n">
-        <v>13</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="82">
@@ -19695,25 +19692,25 @@
         <v>-0.66</v>
       </c>
       <c r="BR82" t="n">
-        <v>-0.48</v>
+        <v>55.71</v>
       </c>
       <c r="BS82" t="n">
-        <v>55.71</v>
+        <v>18</v>
       </c>
       <c r="BT82" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="BU82" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="BV82" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="BW82" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BX82" t="n">
-        <v>11</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="83">
@@ -19925,25 +19922,25 @@
         <v>0.54</v>
       </c>
       <c r="BR83" t="n">
-        <v>-1.23</v>
+        <v>49.32</v>
       </c>
       <c r="BS83" t="n">
-        <v>49.32</v>
+        <v>24</v>
       </c>
       <c r="BT83" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="BU83" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BV83" t="n">
+        <v>14</v>
+      </c>
+      <c r="BW83" t="n">
         <v>11</v>
       </c>
-      <c r="BW83" t="n">
-        <v>14</v>
-      </c>
       <c r="BX83" t="n">
-        <v>11</v>
+        <v>7.49</v>
       </c>
     </row>
     <row r="84">
@@ -20155,25 +20152,25 @@
         <v>1.21</v>
       </c>
       <c r="BR84" t="n">
-        <v>-0.28</v>
+        <v>54.52</v>
       </c>
       <c r="BS84" t="n">
-        <v>54.52</v>
+        <v>15</v>
       </c>
       <c r="BT84" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="BU84" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="BV84" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BW84" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="BX84" t="n">
-        <v>13</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="85">
@@ -20385,25 +20382,25 @@
         <v>-0.06</v>
       </c>
       <c r="BR85" t="n">
-        <v>-1.18</v>
+        <v>49.16</v>
       </c>
       <c r="BS85" t="n">
-        <v>49.16</v>
+        <v>16</v>
       </c>
       <c r="BT85" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="BU85" t="n">
+        <v>11</v>
+      </c>
+      <c r="BV85" t="n">
         <v>8</v>
       </c>
-      <c r="BV85" t="n">
-        <v>11</v>
-      </c>
       <c r="BW85" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="BX85" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -20615,25 +20612,25 @@
         <v>0.55</v>
       </c>
       <c r="BR86" t="n">
-        <v>-1.24</v>
+        <v>53.11</v>
       </c>
       <c r="BS86" t="n">
-        <v>53.11</v>
+        <v>15</v>
       </c>
       <c r="BT86" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="BU86" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="BV86" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="BW86" t="n">
         <v>11</v>
       </c>
       <c r="BX86" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -20845,25 +20842,25 @@
         <v>0.17</v>
       </c>
       <c r="BR87" t="n">
-        <v>-2.35</v>
+        <v>47.95</v>
       </c>
       <c r="BS87" t="n">
-        <v>47.95</v>
+        <v>11</v>
       </c>
       <c r="BT87" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BU87" t="n">
+        <v>9</v>
+      </c>
+      <c r="BV87" t="n">
         <v>8</v>
       </c>
-      <c r="BV87" t="n">
+      <c r="BW87" t="n">
         <v>9</v>
       </c>
-      <c r="BW87" t="n">
-        <v>8</v>
-      </c>
       <c r="BX87" t="n">
-        <v>9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="88">
@@ -21075,25 +21072,25 @@
         <v>0.34</v>
       </c>
       <c r="BR88" t="n">
-        <v>-2.4</v>
+        <v>46.95</v>
       </c>
       <c r="BS88" t="n">
-        <v>46.95</v>
+        <v>12</v>
       </c>
       <c r="BT88" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="BU88" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="BV88" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BW88" t="n">
         <v>8</v>
       </c>
       <c r="BX88" t="n">
-        <v>8</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="89">
@@ -21305,25 +21302,25 @@
         <v>-0.37</v>
       </c>
       <c r="BR89" t="n">
-        <v>-0.61</v>
+        <v>59.57</v>
       </c>
       <c r="BS89" t="n">
-        <v>59.57</v>
+        <v>10</v>
       </c>
       <c r="BT89" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU89" t="n">
         <v>10</v>
       </c>
-      <c r="BU89" t="n">
-        <v>7</v>
-      </c>
       <c r="BV89" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BW89" t="n">
         <v>9</v>
       </c>
       <c r="BX89" t="n">
-        <v>9</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="90">
@@ -21535,25 +21532,25 @@
         <v>-0.35</v>
       </c>
       <c r="BR90" t="n">
-        <v>-0.68</v>
+        <v>54.72</v>
       </c>
       <c r="BS90" t="n">
-        <v>54.72</v>
+        <v>11</v>
       </c>
       <c r="BT90" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU90" t="n">
         <v>11</v>
       </c>
-      <c r="BU90" t="n">
-        <v>7</v>
-      </c>
       <c r="BV90" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BW90" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BX90" t="n">
-        <v>9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="91">
@@ -21765,25 +21762,25 @@
         <v>0.64</v>
       </c>
       <c r="BR91" t="n">
-        <v>-0.17</v>
+        <v>57.7</v>
       </c>
       <c r="BS91" t="n">
-        <v>57.7</v>
+        <v>11</v>
       </c>
       <c r="BT91" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BU91" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="BV91" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="BW91" t="n">
         <v>9</v>
       </c>
       <c r="BX91" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92">
@@ -21995,25 +21992,25 @@
         <v>1.73</v>
       </c>
       <c r="BR92" t="n">
-        <v>-1.57</v>
+        <v>49.36</v>
       </c>
       <c r="BS92" t="n">
-        <v>49.36</v>
+        <v>11</v>
       </c>
       <c r="BT92" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BU92" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="BV92" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="BW92" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BX92" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -22225,25 +22222,25 @@
         <v>-0.96</v>
       </c>
       <c r="BR93" t="n">
-        <v>-0.18</v>
+        <v>60.68</v>
       </c>
       <c r="BS93" t="n">
-        <v>60.68</v>
+        <v>15</v>
       </c>
       <c r="BT93" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BU93" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BV93" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="BW93" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="BX93" t="n">
-        <v>9</v>
+        <v>7.49</v>
       </c>
     </row>
     <row r="94">
@@ -22263,7 +22260,7 @@
         <v>126</v>
       </c>
       <c r="F94" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G94" t="s">
         <v>91</v>
@@ -22455,30 +22452,30 @@
         <v>2.24</v>
       </c>
       <c r="BR94" t="n">
-        <v>-1.14</v>
+        <v>52.65</v>
       </c>
       <c r="BS94" t="n">
-        <v>52.65</v>
+        <v>11</v>
       </c>
       <c r="BT94" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="BU94" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BV94" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="BW94" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BX94" t="n">
-        <v>7</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B95" t="s">
         <v>77</v>
@@ -22685,30 +22682,30 @@
         <v>-2.46</v>
       </c>
       <c r="BR95" t="n">
-        <v>-4.34</v>
+        <v>27.23</v>
       </c>
       <c r="BS95" t="n">
-        <v>27.23</v>
+        <v>11</v>
       </c>
       <c r="BT95" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BU95" t="n">
+        <v>8</v>
+      </c>
+      <c r="BV95" t="n">
+        <v>4</v>
+      </c>
+      <c r="BW95" t="n">
         <v>7</v>
       </c>
-      <c r="BV95" t="n">
-        <v>8</v>
-      </c>
-      <c r="BW95" t="n">
-        <v>4</v>
-      </c>
       <c r="BX95" t="n">
-        <v>7</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B96" t="s">
         <v>77</v>
@@ -22915,30 +22912,30 @@
         <v>0.3</v>
       </c>
       <c r="BR96" t="n">
-        <v>-1.54</v>
+        <v>51.99</v>
       </c>
       <c r="BS96" t="n">
-        <v>51.99</v>
+        <v>9</v>
       </c>
       <c r="BT96" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU96" t="n">
         <v>9</v>
       </c>
-      <c r="BU96" t="n">
+      <c r="BV96" t="n">
         <v>7</v>
       </c>
-      <c r="BV96" t="n">
+      <c r="BW96" t="n">
         <v>9</v>
       </c>
-      <c r="BW96" t="n">
-        <v>7</v>
-      </c>
       <c r="BX96" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B97" t="s">
         <v>88</v>
@@ -22953,7 +22950,7 @@
         <v>126</v>
       </c>
       <c r="F97" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G97" t="s">
         <v>91</v>
@@ -23145,30 +23142,30 @@
         <v>-1.36</v>
       </c>
       <c r="BR97" t="n">
-        <v>-1.87</v>
+        <v>45.36</v>
       </c>
       <c r="BS97" t="n">
-        <v>45.36</v>
+        <v>13</v>
       </c>
       <c r="BT97" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="BU97" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BV97" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="BW97" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BX97" t="n">
-        <v>11</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B98" t="s">
         <v>77</v>
@@ -23375,30 +23372,30 @@
         <v>-0.8</v>
       </c>
       <c r="BR98" t="n">
-        <v>-4.37</v>
+        <v>32.5</v>
       </c>
       <c r="BS98" t="n">
-        <v>32.5</v>
+        <v>17</v>
       </c>
       <c r="BT98" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="BU98" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BV98" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BW98" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="BX98" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B99" t="s">
         <v>88</v>
@@ -23410,7 +23407,7 @@
         <v>13</v>
       </c>
       <c r="E99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F99" t="s">
         <v>79</v>
@@ -23605,30 +23602,30 @@
         <v>-2.13</v>
       </c>
       <c r="BR99" t="n">
-        <v>-4.84</v>
+        <v>21.93</v>
       </c>
       <c r="BS99" t="n">
-        <v>21.93</v>
+        <v>17</v>
       </c>
       <c r="BT99" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="BU99" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BV99" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="BW99" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BX99" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100" t="s">
         <v>88</v>
@@ -23835,30 +23832,30 @@
         <v>-1.9</v>
       </c>
       <c r="BR100" t="n">
-        <v>-4.87</v>
+        <v>26.45</v>
       </c>
       <c r="BS100" t="n">
-        <v>26.45</v>
+        <v>12</v>
       </c>
       <c r="BT100" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="BU100" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="BV100" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="BW100" t="n">
+        <v>10</v>
+      </c>
+      <c r="BX100" t="n">
         <v>6</v>
-      </c>
-      <c r="BX100" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B101" t="s">
         <v>88</v>
@@ -23870,10 +23867,10 @@
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F101" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G101" t="s">
         <v>80</v>
@@ -24065,30 +24062,30 @@
         <v>-0.37</v>
       </c>
       <c r="BR101" t="n">
-        <v>-2.17</v>
+        <v>43.79</v>
       </c>
       <c r="BS101" t="n">
-        <v>43.79</v>
+        <v>10</v>
       </c>
       <c r="BT101" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="BU101" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="BV101" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW101" t="n">
         <v>11</v>
       </c>
-      <c r="BW101" t="n">
-        <v>9</v>
-      </c>
       <c r="BX101" t="n">
-        <v>11</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B102" t="s">
         <v>77</v>
@@ -24295,30 +24292,30 @@
         <v>-1.12</v>
       </c>
       <c r="BR102" t="n">
-        <v>-0.78</v>
+        <v>43.91</v>
       </c>
       <c r="BS102" t="n">
-        <v>43.91</v>
+        <v>15</v>
       </c>
       <c r="BT102" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="BU102" t="n">
+        <v>10</v>
+      </c>
+      <c r="BV102" t="n">
+        <v>4</v>
+      </c>
+      <c r="BW102" t="n">
         <v>5</v>
       </c>
-      <c r="BV102" t="n">
-        <v>10</v>
-      </c>
-      <c r="BW102" t="n">
-        <v>4</v>
-      </c>
       <c r="BX102" t="n">
-        <v>5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B103" t="s">
         <v>88</v>
@@ -24525,30 +24522,30 @@
         <v>-0.35</v>
       </c>
       <c r="BR103" t="n">
-        <v>0.17</v>
+        <v>56.48</v>
       </c>
       <c r="BS103" t="n">
-        <v>56.48</v>
+        <v>11</v>
       </c>
       <c r="BT103" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="BU103" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="BV103" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="BW103" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BX103" t="n">
-        <v>7</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B104" t="s">
         <v>88</v>
@@ -24755,16 +24752,16 @@
         <v>1.21</v>
       </c>
       <c r="BR104" t="n">
-        <v>-1.34</v>
+        <v>45.63</v>
       </c>
       <c r="BS104" t="n">
-        <v>45.63</v>
+        <v>7</v>
       </c>
       <c r="BT104" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="BU104" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BV104" t="n">
         <v>6</v>
@@ -24773,12 +24770,12 @@
         <v>6</v>
       </c>
       <c r="BX104" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B105" t="s">
         <v>77</v>
@@ -24985,30 +24982,30 @@
         <v>-0.45</v>
       </c>
       <c r="BR105" t="n">
-        <v>-4.13</v>
+        <v>24.45</v>
       </c>
       <c r="BS105" t="n">
-        <v>24.45</v>
+        <v>13</v>
       </c>
       <c r="BT105" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="BU105" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="BV105" t="n">
+        <v>7</v>
+      </c>
+      <c r="BW105" t="n">
         <v>9</v>
       </c>
-      <c r="BW105" t="n">
-        <v>7</v>
-      </c>
       <c r="BX105" t="n">
-        <v>9</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B106" t="s">
         <v>88</v>
@@ -25215,30 +25212,30 @@
         <v>0.21</v>
       </c>
       <c r="BR106" t="n">
-        <v>-1.69</v>
+        <v>46.54</v>
       </c>
       <c r="BS106" t="n">
-        <v>46.54</v>
+        <v>9</v>
       </c>
       <c r="BT106" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="BU106" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="BV106" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BW106" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BX106" t="n">
-        <v>8</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B107" t="s">
         <v>77</v>
@@ -25445,30 +25442,30 @@
         <v>-1.9</v>
       </c>
       <c r="BR107" t="n">
-        <v>-4.22</v>
+        <v>27.44</v>
       </c>
       <c r="BS107" t="n">
-        <v>27.44</v>
+        <v>20</v>
       </c>
       <c r="BT107" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="BU107" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="BV107" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="BW107" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BX107" t="n">
-        <v>7</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B108" t="s">
         <v>88</v>
@@ -25675,30 +25672,30 @@
         <v>-0.23</v>
       </c>
       <c r="BR108" t="n">
-        <v>-0.41</v>
+        <v>55.9</v>
       </c>
       <c r="BS108" t="n">
-        <v>55.9</v>
+        <v>10</v>
       </c>
       <c r="BT108" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="BU108" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="BV108" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="BW108" t="n">
+        <v>9</v>
+      </c>
+      <c r="BX108" t="n">
         <v>6</v>
-      </c>
-      <c r="BX108" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B109" t="s">
         <v>77</v>
@@ -25905,25 +25902,25 @@
         <v>-0.8</v>
       </c>
       <c r="BR109" t="n">
-        <v>-2.88</v>
+        <v>43.33</v>
       </c>
       <c r="BS109" t="n">
-        <v>43.33</v>
+        <v>9</v>
       </c>
       <c r="BT109" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="BU109" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="BV109" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="BW109" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BX109" t="n">
-        <v>7</v>
+        <v>3.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: shiny, add: t.test, shapiro, diff
</commit_message>
<xml_diff>
--- a/scripts/_misc/Data_SAS_fixed.xlsx
+++ b/scripts/_misc/Data_SAS_fixed.xlsx
@@ -2689,9 +2689,7 @@
       <c r="BW8" t="n">
         <v>14</v>
       </c>
-      <c r="BX8" t="n">
-        <v>3</v>
-      </c>
+      <c r="BX8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -3839,9 +3837,7 @@
       <c r="BW13" t="n">
         <v>10</v>
       </c>
-      <c r="BX13" t="n">
-        <v>0.38</v>
-      </c>
+      <c r="BX13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -4069,9 +4065,7 @@
       <c r="BW14" t="n">
         <v>18</v>
       </c>
-      <c r="BX14" t="n">
-        <v>0.38</v>
-      </c>
+      <c r="BX14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -4759,9 +4753,7 @@
       <c r="BW17" t="n">
         <v>15</v>
       </c>
-      <c r="BX17" t="n">
-        <v>0.56</v>
-      </c>
+      <c r="BX17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -7059,9 +7051,7 @@
       <c r="BW27" t="n">
         <v>15</v>
       </c>
-      <c r="BX27" t="n">
-        <v>4.5</v>
-      </c>
+      <c r="BX27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -9129,9 +9119,7 @@
       <c r="BW36" t="n">
         <v>13</v>
       </c>
-      <c r="BX36" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="BX36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -15109,9 +15097,7 @@
       <c r="BW62" t="n">
         <v>8</v>
       </c>
-      <c r="BX62" t="n">
-        <v>3</v>
-      </c>
+      <c r="BX62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
@@ -16259,9 +16245,7 @@
       <c r="BW67" t="n">
         <v>11</v>
       </c>
-      <c r="BX67" t="n">
-        <v>0.38</v>
-      </c>
+      <c r="BX67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
@@ -16489,9 +16473,7 @@
       <c r="BW68" t="n">
         <v>12</v>
       </c>
-      <c r="BX68" t="n">
-        <v>0.38</v>
-      </c>
+      <c r="BX68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
@@ -17179,9 +17161,7 @@
       <c r="BW71" t="n">
         <v>12</v>
       </c>
-      <c r="BX71" t="n">
-        <v>0.56</v>
-      </c>
+      <c r="BX71"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
@@ -19479,9 +19459,7 @@
       <c r="BW81" t="n">
         <v>13</v>
       </c>
-      <c r="BX81" t="n">
-        <v>4.5</v>
-      </c>
+      <c r="BX81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
@@ -21549,9 +21527,7 @@
       <c r="BW90" t="n">
         <v>9</v>
       </c>
-      <c r="BX90" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="BX90"/>
     </row>
     <row r="91">
       <c r="A91" t="s">

</xml_diff>